<commit_message>
chore: update input file of TDD case3 to last version
Updated input files used to run the test case 3 for the TDD to the last version already available in folder ..\source_code\input_files\input_file_template.

modified:   ../TDD_examples/CASE_3_HTS_HVDC/conductor_1_coupling.xlsx
modified:   ../TDD_examples/CASE_3_HTS_HVDC/conductor_1_input.xlsx
modified:   ../TDD_examples/CASE_3_HTS_HVDC/conductor_1_operation.xlsx
modified:   ../TDD_examples/CASE_3_HTS_HVDC/conductor_definition.xlsx
modified:   ../TDD_examples/CASE_3_HTS_HVDC/conductor_diagnostic.xlsx
modified:   ../TDD_examples/CASE_3_HTS_HVDC/conductor_grid.xlsx
modified:   ../TDD_examples/CASE_3_HTS_HVDC/environment_input.xlsx
</commit_message>
<xml_diff>
--- a/TDD_examples/CASE_3_HTS_HVDC/conductor_diagnostic.xlsx
+++ b/TDD_examples/CASE_3_HTS_HVDC/conductor_diagnostic.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/SC2_38/Description_of_Components/HTS_best_paths/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\TDD_examples\CASE_3_HTS_HVDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="164" documentId="13_ncr:1_{0D969C7C-59B6-4D41-9C8A-C3C1D111D96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{489709C2-885C-407A-8761-21B3910AF5C1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96913D03-6B9E-4790-BBA4-D969F15C6EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5190" yWindow="4200" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Space" sheetId="1" r:id="rId1"/>
-    <sheet name="Time" sheetId="2" r:id="rId2"/>
+    <sheet name="Spatial_distribution" sheetId="1" r:id="rId1"/>
+    <sheet name="Time_evolution" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
@@ -204,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -220,48 +220,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -286,9 +269,9 @@
     <sheetNames>
       <sheetName val="CONDUCTOR_files"/>
       <sheetName val="CONDUCTOR_input"/>
-      <sheetName val="CONDUCTOR_COUPLING"/>
+      <sheetName val="CONDUCTOR_operation"/>
+      <sheetName val="CONDUCTOR_coupling"/>
       <sheetName val="General Format"/>
-      <sheetName val="CONDUCTOR"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -303,7 +286,7 @@
       </sheetData>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
-      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="3"/>
       <sheetData sheetId="4" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
@@ -610,66 +593,66 @@
       <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.54296875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.90625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="4"/>
+    <col min="1" max="1" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="str">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="str">
         <f>[1]CONDUCTOR_files!$A$1</f>
         <v>CONDUCTOR</v>
       </c>
-      <c r="B1" s="16">
+      <c r="B1" s="12">
         <f>SUM(E2:G2)</f>
         <v>1</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="10">
+      <c r="E1" s="8">
         <f>[1]CONDUCTOR_files!E$1</f>
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="10">
+      <c r="E2" s="8">
         <f>IF(E$1 &gt; 0,1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="str">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="str">
         <f>[2]TRANSIENT!A$2</f>
         <v>Variable name</v>
       </c>
-      <c r="B3" s="9" t="str">
+      <c r="B3" s="7" t="str">
         <f>[2]TRANSIENT!B$2</f>
         <v>Unit</v>
       </c>
-      <c r="C3" s="9" t="str">
+      <c r="C3" s="7" t="str">
         <f>[2]TRANSIENT!C$2</f>
         <v>Variable type</v>
       </c>
-      <c r="D3" s="9" t="str">
+      <c r="D3" s="7" t="str">
         <f>[2]TRANSIENT!D$2</f>
         <v>Note/comments</v>
       </c>
-      <c r="E3" s="10" t="str">
+      <c r="E3" s="8" t="str">
         <f>_xlfn.TEXTJOIN("_",,$A$1,E$1)</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -678,13 +661,13 @@
       <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="12">
+      <c r="D4" s="10"/>
+      <c r="E4" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -693,12 +676,12 @@
       <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -707,12 +690,12 @@
       <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="11">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -721,12 +704,12 @@
       <c r="C7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="11">
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -735,12 +718,12 @@
       <c r="C8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="11">
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -749,12 +732,12 @@
       <c r="C9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="11">
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -763,12 +746,12 @@
       <c r="C10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="11">
         <v>2000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="13" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -777,12 +760,12 @@
       <c r="C11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="11">
         <v>4000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="13" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -791,12 +774,12 @@
       <c r="C12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="11">
         <v>6000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="13" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -805,12 +788,12 @@
       <c r="C13" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="11">
         <v>8000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="13" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -819,12 +802,12 @@
       <c r="C14" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="11">
         <v>10000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="13" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -833,12 +816,12 @@
       <c r="C15" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="11">
         <v>12000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="13" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -847,12 +830,12 @@
       <c r="C16" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="11">
         <v>14000</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="13" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>33</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -861,12 +844,12 @@
       <c r="C17" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="11">
         <v>16000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="13" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -875,7 +858,7 @@
       <c r="C18" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="11">
         <v>18000</v>
       </c>
     </row>
@@ -895,330 +878,330 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="4"/>
+    <col min="5" max="5" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="str">
-        <f>Space!A1</f>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="str">
+        <f>Spatial_distribution!A1</f>
         <v>CONDUCTOR</v>
       </c>
-      <c r="B1" s="10">
-        <f>Space!B1</f>
-        <v>1</v>
-      </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="10">
-        <f>Space!E1</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="10">
-        <f>Space!E2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="str">
-        <f>Space!A3</f>
+      <c r="B1" s="8">
+        <f>Spatial_distribution!B1</f>
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="8">
+        <f>Spatial_distribution!E1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="8">
+        <f>Spatial_distribution!E2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="str">
+        <f>Spatial_distribution!A3</f>
         <v>Variable name</v>
       </c>
-      <c r="B3" s="8" t="str">
-        <f>Space!B3</f>
+      <c r="B3" s="6" t="str">
+        <f>Spatial_distribution!B3</f>
         <v>Unit</v>
       </c>
-      <c r="C3" s="8" t="str">
-        <f>Space!C3</f>
+      <c r="C3" s="6" t="str">
+        <f>Spatial_distribution!C3</f>
         <v>Variable type</v>
       </c>
-      <c r="D3" s="8" t="str">
-        <f>Space!D3</f>
+      <c r="D3" s="6" t="str">
+        <f>Spatial_distribution!D3</f>
         <v>Note/comments</v>
       </c>
-      <c r="E3" s="10" t="str">
-        <f>Space!E3</f>
+      <c r="E3" s="8" t="str">
+        <f>Spatial_distribution!E3</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="12">
+      <c r="B6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="12">
+      <c r="B7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="12">
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="12">
+      <c r="B10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="12">
+      <c r="B11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="5">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="12">
+      <c r="B12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="5">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="12">
+      <c r="B13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="5">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="12">
+      <c r="B14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="12">
+      <c r="B15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="5">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="12">
+      <c r="B16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="5">
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="12">
+      <c r="B17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="5">
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="17">
+      <c r="B18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="11">
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="17">
+      <c r="B19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="11">
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="12">
+      <c r="B20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="5">
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="17">
+      <c r="B21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="11">
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" s="17">
+      <c r="B22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="11">
         <v>99</v>
       </c>
     </row>

</xml_diff>